<commit_message>
update with better code
</commit_message>
<xml_diff>
--- a/data/output/tests.xlsx
+++ b/data/output/tests.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eugeniopaglino/Dropbox/Upenn/GitHub/NG-decomposition/data/output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F11BB4C-0127-C041-A3CE-CD48AFB5E278}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21DBEEF8-F1D0-AE47-9D60-8A38F81418E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="19200" firstSheet="1" activeTab="1" xr2:uid="{A7B85AE1-5B9D-FF48-8B3F-4D6C68F4C099}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="30720" windowHeight="17480" firstSheet="32" activeTab="41" xr2:uid="{A7B85AE1-5B9D-FF48-8B3F-4D6C68F4C099}"/>
   </bookViews>
   <sheets>
     <sheet name="allData" sheetId="2" r:id="rId1"/>
@@ -787,14 +787,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -32079,7 +32078,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0D1DE24-9631-144E-BD03-FF1A0BE0A147}">
   <dimension ref="A1:O20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
@@ -61322,8 +61321,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63CFC58D-B57B-FB44-BD10-C59F43014CC7}">
   <dimension ref="A1:J120"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="B112" sqref="B112:B116"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="J119" sqref="J119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -62870,8 +62869,8 @@
         <f>AVERAGE(B$8:B$13)</f>
         <v>0.34884727831098417</v>
       </c>
-      <c r="J98" s="4">
-        <f t="shared" ref="J98:J99" si="17">AVERAGE(I$96,I$100)</f>
+      <c r="J98">
+        <f t="shared" ref="J98" si="17">AVERAGE(I$96,I$100)</f>
         <v>0.19634138648806498</v>
       </c>
     </row>

</xml_diff>